<commit_message>
Fix on invo_professional_team to replace -1 values with NULL
</commit_message>
<xml_diff>
--- a/docs/admin/ssd_repo_tree.xlsx
+++ b/docs/admin/ssd_repo_tree.xlsx
@@ -465,11 +465,6 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>result_matrix.csv</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
           <t>poetry.lock</t>
         </is>
       </c>
@@ -1012,12 +1007,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_v1.1.5_1_20240704.sql</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp.sql</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_version_log.csv</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp_Bradford.sql</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719.sql</t>
         </is>
       </c>
     </row>
@@ -1029,45 +1029,105 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="V13" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -1750,10 +1810,15 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -3454,10 +3519,15 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -3587,10 +3657,15 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="J52" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -3634,10 +3709,15 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="J53" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -3663,45 +3743,105 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="K55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="U55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="V55" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -4201,12 +4341,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_v1.1.5_1_20240704.sql</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp.sql</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_version_log.csv</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp_Bradford.sql</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719.sql</t>
         </is>
       </c>
     </row>
@@ -4218,45 +4363,105 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="K60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr">
+      <c r="U60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
+      <c r="V60" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -4270,45 +4475,105 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="K61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr">
+      <c r="U61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J61" t="inlineStr">
+      <c r="V61" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -7313,10 +7578,15 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr">
+      <c r="J100" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -7360,10 +7630,15 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr">
+      <c r="J101" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -7493,10 +7768,15 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="J105" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -7540,10 +7820,15 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
+          <t>result_matrix.csv</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
           <t>run2_unique_id_list.csv</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr">
+      <c r="J106" t="inlineStr">
         <is>
           <t>ssd_person_personID_testing_escc_result_matrix_2.csv</t>
         </is>
@@ -7615,12 +7900,17 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_v1.1.5_1_20240704.sql</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp.sql</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_version_log.csv</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp_Bradford.sql</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719.sql</t>
         </is>
       </c>
     </row>
@@ -7632,45 +7922,105 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
+      <c r="D112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D112" t="inlineStr">
+      <c r="E112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr">
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
+      <c r="K112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G112" t="inlineStr">
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H112" t="inlineStr">
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I112" t="inlineStr">
+      <c r="U112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J112" t="inlineStr">
+      <c r="V112" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -8170,45 +8520,105 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
+      <c r="D116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr">
+      <c r="E116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr">
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr">
+      <c r="K116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G116" t="inlineStr">
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H116" t="inlineStr">
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I116" t="inlineStr">
+      <c r="U116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J116" t="inlineStr">
+      <c r="V116" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -8708,12 +9118,17 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_v1.1.5_1_20240704.sql</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp.sql</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>liquidlogic_sqlserver_version_log.csv</t>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719_temp_Bradford.sql</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240719.sql</t>
         </is>
       </c>
     </row>
@@ -8725,45 +9140,105 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="D121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D121" t="inlineStr">
+      <c r="E121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
+      <c r="K121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G121" t="inlineStr">
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H121" t="inlineStr">
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I121" t="inlineStr">
+      <c r="U121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J121" t="inlineStr">
+      <c r="V121" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>
@@ -8777,45 +9252,105 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718 - pre updates removal.sql</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
           <t>liquidlogic_sqlserver_temp_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr">
+      <c r="D122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625.sql</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr">
+      <c r="E122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628.sql</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr">
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716.sql</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715_temp.sql</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240715.sql</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718_temp.sql</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.3_1_20240627.sql</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr">
+      <c r="K122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.4_1_20240628_temp.sql</t>
         </is>
       </c>
-      <c r="G122" t="inlineStr">
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240718.sql</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.7_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710_TEMP.sql</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.9_1_20240717.sql</t>
+        </is>
+      </c>
+      <c r="P122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.6_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.8_1_20240716_temp.sql</t>
+        </is>
+      </c>
+      <c r="R122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_v1.1.1_1_20240625_VIEWS.sql</t>
         </is>
       </c>
-      <c r="H122" t="inlineStr">
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>liquidlogic_sqlserver_v1.1.5_1_20240710.sql</t>
+        </is>
+      </c>
+      <c r="T122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK2.sql</t>
         </is>
       </c>
-      <c r="I122" t="inlineStr">
+      <c r="U122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_temp_ssd_test060524.sql</t>
         </is>
       </c>
-      <c r="J122" t="inlineStr">
+      <c r="V122" t="inlineStr">
         <is>
           <t>liquidlogic_sqlserver_perm_ssd BAK1.sql</t>
         </is>

</xml_diff>